<commit_message>
Added the sequence diagram to the DD
</commit_message>
<xml_diff>
--- a/Effort/EffortGianmarcoAccordiDD.xlsx
+++ b/Effort/EffortGianmarcoAccordiDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianmarco Accordi\Documents\Project-INGSW2\AbboAccordiBonetti\Effort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E652FD6-C965-4029-8761-9EB885930A04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1895E56F-9181-403A-B2A4-0C6E85CAA5F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Massimiliano Bonetti</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>0.5</t>
+  </si>
+  <si>
+    <t>26.5</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -469,8 +472,8 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>20</v>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>